<commit_message>
added the merger and adding_ltp in main_scanner
</commit_message>
<xml_diff>
--- a/csv_files/merged_data_with_ltp.xlsx
+++ b/csv_files/merged_data_with_ltp.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imadc\PycharmProjects\fwdproject\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E8F3F16-5705-4EB1-81B5-9BC4AD2EC236}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27B3F173-F746-4888-8DAF-E18D33AA3E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA25306F-F9BE-412F-841E-D4614913F7ED}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{107A90F5-14F5-4363-A9C9-721FA99E1B35}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -26,6 +26,12 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+  <si>
+    <t>45_days</t>
+  </si>
+  <si>
+    <t>15_days</t>
+  </si>
   <si>
     <t>stock</t>
   </si>
@@ -46,12 +52,6 @@
   </si>
   <si>
     <t>ltp</t>
-  </si>
-  <si>
-    <t>45 days</t>
-  </si>
-  <si>
-    <t>15 days</t>
   </si>
 </sst>
 </file>
@@ -185,14 +185,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -515,22 +515,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9D1987-FA67-41BE-8B57-630B946ACCC3}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{32D1834C-BADF-4B00-9F93-85D09A23434C}">
   <dimension ref="A1:T7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+      <selection activeCell="P12" sqref="P12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="13.77734375" customWidth="1"/>
-    <col min="2" max="2" width="10.21875" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
       <c r="C1" s="11" t="s">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
@@ -541,7 +537,7 @@
       <c r="J1" s="12"/>
       <c r="K1" s="13"/>
       <c r="L1" s="11" t="s">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="M1" s="12"/>
       <c r="N1" s="12"/>
@@ -552,74 +548,74 @@
       <c r="S1" s="12"/>
       <c r="T1" s="13"/>
     </row>
-    <row r="2" spans="1:20" s="6" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:20" s="8" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="9">
         <v>0</v>
       </c>
-      <c r="B2" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="7">
+      <c r="D2" s="8">
+        <v>0.23599999999999999</v>
+      </c>
+      <c r="E2" s="8">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="F2" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="G2" s="8">
+        <v>0.61799999999999999</v>
+      </c>
+      <c r="H2" s="8">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="I2" s="8">
+        <v>1</v>
+      </c>
+      <c r="J2" s="8">
+        <v>1.236</v>
+      </c>
+      <c r="K2" s="10">
+        <v>1.6180000000000001</v>
+      </c>
+      <c r="L2" s="9">
         <v>0</v>
       </c>
-      <c r="D2" s="6">
+      <c r="M2" s="8">
         <v>0.23599999999999999</v>
       </c>
-      <c r="E2" s="6">
+      <c r="N2" s="8">
         <v>0.38200000000000001</v>
       </c>
-      <c r="F2" s="6">
+      <c r="O2" s="8">
         <v>0.5</v>
       </c>
-      <c r="G2" s="6">
+      <c r="P2" s="8">
         <v>0.61799999999999999</v>
       </c>
-      <c r="H2" s="6">
+      <c r="Q2" s="8">
         <v>0.78600000000000003</v>
       </c>
-      <c r="I2" s="6">
+      <c r="R2" s="8">
         <v>1</v>
       </c>
-      <c r="J2" s="6">
+      <c r="S2" s="8">
         <v>1.236</v>
       </c>
-      <c r="K2" s="8">
-        <v>1.6180000000000001</v>
-      </c>
-      <c r="L2" s="7">
-        <v>0</v>
-      </c>
-      <c r="M2" s="6">
-        <v>0.23599999999999999</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="O2" s="6">
-        <v>0.5</v>
-      </c>
-      <c r="P2" s="6">
-        <v>0.61799999999999999</v>
-      </c>
-      <c r="Q2" s="6">
-        <v>0.78600000000000003</v>
-      </c>
-      <c r="R2" s="6">
-        <v>1</v>
-      </c>
-      <c r="S2" s="6">
-        <v>1.236</v>
-      </c>
-      <c r="T2" s="8">
+      <c r="T2" s="10">
         <v>1.6180000000000001</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3">
-        <v>602.79999999999995</v>
+        <v>601.85</v>
       </c>
       <c r="C3" s="1">
         <v>515.54999999999995</v>
@@ -639,7 +635,7 @@
       <c r="H3">
         <v>630.27</v>
       </c>
-      <c r="I3" s="9">
+      <c r="I3" s="3">
         <v>661.5</v>
       </c>
       <c r="J3">
@@ -666,7 +662,7 @@
       <c r="Q3">
         <v>639.37</v>
       </c>
-      <c r="R3" s="9">
+      <c r="R3" s="3">
         <v>661.5</v>
       </c>
       <c r="S3">
@@ -678,10 +674,10 @@
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>4953.25</v>
+        <v>4890</v>
       </c>
       <c r="C4" s="1">
         <v>4195.55</v>
@@ -701,7 +697,7 @@
       <c r="H4">
         <v>4794.05</v>
       </c>
-      <c r="I4" s="9">
+      <c r="I4" s="3">
         <v>4957</v>
       </c>
       <c r="J4">
@@ -728,7 +724,7 @@
       <c r="Q4">
         <v>4865.43</v>
       </c>
-      <c r="R4" s="9">
+      <c r="R4" s="3">
         <v>4957</v>
       </c>
       <c r="S4">
@@ -740,12 +736,12 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>23913.599999999999</v>
-      </c>
-      <c r="C5" s="10">
+        <v>24340.400000000001</v>
+      </c>
+      <c r="C5" s="4">
         <v>22000</v>
       </c>
       <c r="D5">
@@ -772,7 +768,7 @@
       <c r="K5" s="2">
         <v>25516.240000000002</v>
       </c>
-      <c r="L5" s="10">
+      <c r="L5" s="4">
         <v>22000</v>
       </c>
       <c r="M5">
@@ -802,12 +798,12 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>175.8</v>
-      </c>
-      <c r="C6" s="10">
+        <v>173.25</v>
+      </c>
+      <c r="C6" s="4">
         <v>155</v>
       </c>
       <c r="D6">
@@ -834,7 +830,7 @@
       <c r="K6" s="2">
         <v>200.14</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="4">
         <v>155</v>
       </c>
       <c r="M6">
@@ -864,63 +860,63 @@
     </row>
     <row r="7" spans="1:20" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>233.85</v>
-      </c>
-      <c r="C7" s="3">
+        <v>225.4</v>
+      </c>
+      <c r="C7" s="5">
         <v>212.45</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="6">
         <v>220.13</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="6">
         <v>224.88</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="6">
         <v>228.72</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="6">
         <v>232.57</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="6">
         <v>238.03</v>
       </c>
-      <c r="I7" s="4">
+      <c r="I7" s="6">
         <v>245</v>
       </c>
-      <c r="J7" s="4">
+      <c r="J7" s="6">
         <v>252.68</v>
       </c>
-      <c r="K7" s="5">
+      <c r="K7" s="7">
         <v>265.12</v>
       </c>
-      <c r="L7" s="3">
+      <c r="L7" s="5">
         <v>215.4</v>
       </c>
-      <c r="M7" s="4">
+      <c r="M7" s="6">
         <v>220.64</v>
       </c>
-      <c r="N7" s="4">
+      <c r="N7" s="6">
         <v>223.88</v>
       </c>
-      <c r="O7" s="4">
+      <c r="O7" s="6">
         <v>226.5</v>
       </c>
-      <c r="P7" s="4">
+      <c r="P7" s="6">
         <v>229.12</v>
       </c>
-      <c r="Q7" s="4">
+      <c r="Q7" s="6">
         <v>232.85</v>
       </c>
-      <c r="R7" s="4">
+      <c r="R7" s="6">
         <v>237.6</v>
       </c>
-      <c r="S7" s="4">
+      <c r="S7" s="6">
         <v>242.84</v>
       </c>
-      <c r="T7" s="5">
+      <c r="T7" s="7">
         <v>251.32</v>
       </c>
     </row>

</xml_diff>

<commit_message>
final commit before project refactoring
</commit_message>
<xml_diff>
--- a/csv_files/merged_data_with_ltp.xlsx
+++ b/csv_files/merged_data_with_ltp.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\imadc\PycharmProjects\fwdproject\csv_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA200E3-990F-43EA-81FF-7AFA1566A504}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB11B30B-1A07-4863-8694-5DCF68078918}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{DB6DE79E-2F82-47EF-A67F-10CB8D26D03C}"/>
   </bookViews>
@@ -615,7 +615,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -625,12 +625,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -727,7 +721,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -740,8 +734,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1068,7 +1060,7 @@
   <dimension ref="A1:T187"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1078,28 +1070,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="C1" s="14" t="s">
+      <c r="C1" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="14" t="s">
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
+      <c r="G1" s="13"/>
+      <c r="H1" s="13"/>
+      <c r="I1" s="13"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
-      <c r="T1" s="16"/>
+      <c r="M1" s="13"/>
+      <c r="N1" s="13"/>
+      <c r="O1" s="13"/>
+      <c r="P1" s="13"/>
+      <c r="Q1" s="13"/>
+      <c r="R1" s="13"/>
+      <c r="S1" s="13"/>
+      <c r="T1" s="14"/>
     </row>
     <row r="2" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
@@ -1168,7 +1160,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>603.6</v>
+        <v>614.54999999999995</v>
       </c>
       <c r="C3" s="4">
         <v>515.54999999999995</v>
@@ -1230,7 +1222,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>4935.7</v>
+        <v>4913.7</v>
       </c>
       <c r="C4" s="4">
         <v>4195.55</v>
@@ -1292,7 +1284,7 @@
         <v>5</v>
       </c>
       <c r="B5">
-        <v>24609.25</v>
+        <v>24835.95</v>
       </c>
       <c r="C5" s="10">
         <v>22000</v>
@@ -1354,7 +1346,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>173.3</v>
+        <v>176.95</v>
       </c>
       <c r="C6" s="10">
         <v>155</v>
@@ -1416,7 +1408,7 @@
         <v>7</v>
       </c>
       <c r="B7">
-        <v>226.75</v>
+        <v>231.4</v>
       </c>
       <c r="C7" s="4">
         <v>212.45</v>
@@ -1478,7 +1470,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>2306.6</v>
+        <v>2299.8000000000002</v>
       </c>
       <c r="C8" s="4">
         <v>1803</v>
@@ -1540,7 +1532,7 @@
         <v>9</v>
       </c>
       <c r="B9">
-        <v>3098.2</v>
+        <v>3090.6</v>
       </c>
       <c r="C9" s="4">
         <v>2142</v>
@@ -1602,7 +1594,7 @@
         <v>10</v>
       </c>
       <c r="B10">
-        <v>1214.3499999999999</v>
+        <v>1207</v>
       </c>
       <c r="C10" s="4">
         <v>785</v>
@@ -1664,7 +1656,7 @@
         <v>11</v>
       </c>
       <c r="B11">
-        <v>5119.8</v>
+        <v>5055</v>
       </c>
       <c r="C11" s="4">
         <v>4300.3</v>
@@ -1726,7 +1718,7 @@
         <v>12</v>
       </c>
       <c r="B12">
-        <v>526.15</v>
+        <v>526.85</v>
       </c>
       <c r="C12" s="4">
         <v>408.6</v>
@@ -1788,7 +1780,7 @@
         <v>13</v>
       </c>
       <c r="B13">
-        <v>5800.9</v>
+        <v>5814.15</v>
       </c>
       <c r="C13" s="4">
         <v>5201.75</v>
@@ -1850,7 +1842,7 @@
         <v>14</v>
       </c>
       <c r="B14">
-        <v>466.7</v>
+        <v>471.55</v>
       </c>
       <c r="C14" s="4">
         <v>413.95</v>
@@ -1912,7 +1904,7 @@
         <v>15</v>
       </c>
       <c r="B15">
-        <v>175.35</v>
+        <v>176.1</v>
       </c>
       <c r="C15" s="10">
         <v>165.25</v>
@@ -1974,7 +1966,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>3286.85</v>
+        <v>3284</v>
       </c>
       <c r="C16" s="4">
         <v>3078.7</v>
@@ -2036,7 +2028,7 @@
         <v>17</v>
       </c>
       <c r="B17">
-        <v>1810.95</v>
+        <v>1813.8</v>
       </c>
       <c r="C17" s="10">
         <v>1823.55</v>
@@ -2098,7 +2090,7 @@
         <v>18</v>
       </c>
       <c r="B18">
-        <v>6799.4</v>
+        <v>6870</v>
       </c>
       <c r="C18" s="4">
         <v>6473.9</v>
@@ -2160,7 +2152,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>772.45</v>
+        <v>779.5</v>
       </c>
       <c r="C19" s="4">
         <v>710.1</v>
@@ -2222,7 +2214,7 @@
         <v>20</v>
       </c>
       <c r="B20">
-        <v>1123</v>
+        <v>1119.9000000000001</v>
       </c>
       <c r="C20" s="4">
         <v>959</v>
@@ -2284,7 +2276,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>1107</v>
+        <v>1119.4000000000001</v>
       </c>
       <c r="C21" s="4">
         <v>980.35</v>
@@ -2346,7 +2338,7 @@
         <v>22</v>
       </c>
       <c r="B22">
-        <v>7053.75</v>
+        <v>7159.95</v>
       </c>
       <c r="C22" s="4">
         <v>5461.1</v>
@@ -2408,7 +2400,7 @@
         <v>23</v>
       </c>
       <c r="B23">
-        <v>1671.85</v>
+        <v>1688.75</v>
       </c>
       <c r="C23" s="4">
         <v>1539.05</v>
@@ -2470,7 +2462,7 @@
         <v>24</v>
       </c>
       <c r="B24">
-        <v>7680.55</v>
+        <v>7749.8</v>
       </c>
       <c r="C24" s="4">
         <v>6931.25</v>
@@ -2532,7 +2524,7 @@
         <v>25</v>
       </c>
       <c r="B25">
-        <v>2649.8</v>
+        <v>2718</v>
       </c>
       <c r="C25" s="10">
         <v>2407.5</v>
@@ -2594,7 +2586,7 @@
         <v>26</v>
       </c>
       <c r="B26">
-        <v>389.8</v>
+        <v>388</v>
       </c>
       <c r="C26" s="4">
         <v>376.2</v>
@@ -2656,7 +2648,7 @@
         <v>27</v>
       </c>
       <c r="B27">
-        <v>231.05</v>
+        <v>235.75</v>
       </c>
       <c r="C27" s="4">
         <v>211.4</v>
@@ -2718,7 +2710,7 @@
         <v>28</v>
       </c>
       <c r="B28">
-        <v>223.85</v>
+        <v>225.3</v>
       </c>
       <c r="C28" s="4">
         <v>192.75</v>
@@ -2780,7 +2772,7 @@
         <v>29</v>
       </c>
       <c r="B29">
-        <v>1565.25</v>
+        <v>1571.25</v>
       </c>
       <c r="C29" s="4">
         <v>1566.05</v>
@@ -2842,7 +2834,7 @@
         <v>30</v>
       </c>
       <c r="B30">
-        <v>185.6</v>
+        <v>185.85</v>
       </c>
       <c r="C30" s="4">
         <v>137.35</v>
@@ -2904,7 +2896,7 @@
         <v>31</v>
       </c>
       <c r="B31">
-        <v>592.65</v>
+        <v>589.4</v>
       </c>
       <c r="C31" s="4">
         <v>562.70000000000005</v>
@@ -2966,7 +2958,7 @@
         <v>32</v>
       </c>
       <c r="B32">
-        <v>1062.7</v>
+        <v>1067.05</v>
       </c>
       <c r="C32" s="4">
         <v>936.2</v>
@@ -3028,7 +3020,7 @@
         <v>33</v>
       </c>
       <c r="B33">
-        <v>199.65</v>
+        <v>199.95</v>
       </c>
       <c r="C33" s="4">
         <v>135.30000000000001</v>
@@ -3090,7 +3082,7 @@
         <v>34</v>
       </c>
       <c r="B34">
-        <v>281.45</v>
+        <v>285.45</v>
       </c>
       <c r="C34" s="4">
         <v>228.25</v>
@@ -3152,7 +3144,7 @@
         <v>35</v>
       </c>
       <c r="B35">
-        <v>22615.200000000001</v>
+        <v>22771.7</v>
       </c>
       <c r="C35" s="4">
         <v>19500</v>
@@ -3214,7 +3206,7 @@
         <v>36</v>
       </c>
       <c r="B36">
-        <v>451.25</v>
+        <v>457.2</v>
       </c>
       <c r="C36" s="4">
         <v>386.6</v>
@@ -3276,7 +3268,7 @@
         <v>37</v>
       </c>
       <c r="B37">
-        <v>5086.6499999999996</v>
+        <v>5078.8</v>
       </c>
       <c r="C37" s="4">
         <v>4626</v>
@@ -3338,7 +3330,7 @@
         <v>38</v>
       </c>
       <c r="B38">
-        <v>739.55</v>
+        <v>757.8</v>
       </c>
       <c r="C38" s="4">
         <v>590.04999999999995</v>
@@ -3400,7 +3392,7 @@
         <v>39</v>
       </c>
       <c r="B39">
-        <v>448.75</v>
+        <v>454.05</v>
       </c>
       <c r="C39" s="4">
         <v>389</v>
@@ -3462,7 +3454,7 @@
         <v>40</v>
       </c>
       <c r="B40">
-        <v>759.7</v>
+        <v>769.6</v>
       </c>
       <c r="C40" s="4">
         <v>734.2</v>
@@ -3524,7 +3516,7 @@
         <v>41</v>
       </c>
       <c r="B41">
-        <v>374.45</v>
+        <v>376.2</v>
       </c>
       <c r="C41" s="4">
         <v>303</v>
@@ -3586,7 +3578,7 @@
         <v>42</v>
       </c>
       <c r="B42">
-        <v>1216.25</v>
+        <v>1228.8499999999999</v>
       </c>
       <c r="C42" s="4">
         <v>1085.4000000000001</v>
@@ -3648,7 +3640,7 @@
         <v>43</v>
       </c>
       <c r="B43">
-        <v>1329.2</v>
+        <v>1332.95</v>
       </c>
       <c r="C43" s="4">
         <v>1164.55</v>
@@ -3710,7 +3702,7 @@
         <v>44</v>
       </c>
       <c r="B44">
-        <v>382.05</v>
+        <v>387.5</v>
       </c>
       <c r="C44" s="4">
         <v>328.85</v>
@@ -3772,7 +3764,7 @@
         <v>45</v>
       </c>
       <c r="B45">
-        <v>6152.25</v>
+        <v>6284.35</v>
       </c>
       <c r="C45" s="4">
         <v>5125.2</v>
@@ -3834,7 +3826,7 @@
         <v>46</v>
       </c>
       <c r="B46">
-        <v>2396.25</v>
+        <v>2441.65</v>
       </c>
       <c r="C46" s="4">
         <v>2113.8000000000002</v>
@@ -3896,7 +3888,7 @@
         <v>47</v>
       </c>
       <c r="B47">
-        <v>886.3</v>
+        <v>911</v>
       </c>
       <c r="C47" s="4">
         <v>737.85</v>
@@ -3958,7 +3950,7 @@
         <v>48</v>
       </c>
       <c r="B48">
-        <v>1166.6500000000001</v>
+        <v>1173.7</v>
       </c>
       <c r="C48" s="4">
         <v>1103.4000000000001</v>
@@ -4020,7 +4012,7 @@
         <v>49</v>
       </c>
       <c r="B49">
-        <v>322.55</v>
+        <v>323.2</v>
       </c>
       <c r="C49" s="4">
         <v>279.2</v>
@@ -4081,8 +4073,8 @@
       <c r="A50" t="s">
         <v>50</v>
       </c>
-      <c r="B50" s="12">
-        <v>145.69999999999999</v>
+      <c r="B50">
+        <v>147.44999999999999</v>
       </c>
       <c r="C50" s="4">
         <v>142.65</v>
@@ -4111,7 +4103,7 @@
       <c r="K50" s="5">
         <v>183.34</v>
       </c>
-      <c r="L50" s="13">
+      <c r="L50" s="4">
         <v>145.69999999999999</v>
       </c>
       <c r="M50">
@@ -4144,7 +4136,7 @@
         <v>51</v>
       </c>
       <c r="B51">
-        <v>2046.15</v>
+        <v>2041.4</v>
       </c>
       <c r="C51" s="4">
         <v>1780</v>
@@ -4206,7 +4198,7 @@
         <v>52</v>
       </c>
       <c r="B52">
-        <v>547.35</v>
+        <v>554.04999999999995</v>
       </c>
       <c r="C52" s="4">
         <v>516.70000000000005</v>
@@ -4268,7 +4260,7 @@
         <v>53</v>
       </c>
       <c r="B53">
-        <v>2288.6</v>
+        <v>2263.35</v>
       </c>
       <c r="C53" s="4">
         <v>2109.6</v>
@@ -4330,7 +4322,7 @@
         <v>54</v>
       </c>
       <c r="B54">
-        <v>2429.5</v>
+        <v>2443.5</v>
       </c>
       <c r="C54" s="4">
         <v>2108.4</v>
@@ -4392,7 +4384,7 @@
         <v>55</v>
       </c>
       <c r="B55">
-        <v>154.35</v>
+        <v>152.05000000000001</v>
       </c>
       <c r="C55" s="4">
         <v>133.19999999999999</v>
@@ -4454,7 +4446,7 @@
         <v>56</v>
       </c>
       <c r="B56">
-        <v>3902.65</v>
+        <v>3918.3</v>
       </c>
       <c r="C56" s="4">
         <v>3501.25</v>
@@ -4516,7 +4508,7 @@
         <v>57</v>
       </c>
       <c r="B57">
-        <v>6326.95</v>
+        <v>6429</v>
       </c>
       <c r="C57" s="4">
         <v>5213.1000000000004</v>
@@ -4578,7 +4570,7 @@
         <v>58</v>
       </c>
       <c r="B58">
-        <v>796.05</v>
+        <v>800.35</v>
       </c>
       <c r="C58" s="4">
         <v>612.04999999999995</v>
@@ -4640,7 +4632,7 @@
         <v>59</v>
       </c>
       <c r="B59">
-        <v>5787.2</v>
+        <v>5678</v>
       </c>
       <c r="C59" s="4">
         <v>5370</v>
@@ -4702,7 +4694,7 @@
         <v>60</v>
       </c>
       <c r="B60">
-        <v>3842.55</v>
+        <v>3886.45</v>
       </c>
       <c r="C60" s="4">
         <v>3672.1</v>
@@ -4764,7 +4756,7 @@
         <v>61</v>
       </c>
       <c r="B61">
-        <v>2835</v>
+        <v>2875.95</v>
       </c>
       <c r="C61" s="10">
         <v>2924.5</v>
@@ -4826,7 +4818,7 @@
         <v>62</v>
       </c>
       <c r="B62">
-        <v>327.8</v>
+        <v>330.1</v>
       </c>
       <c r="C62" s="4">
         <v>270.8</v>
@@ -4888,7 +4880,7 @@
         <v>63</v>
       </c>
       <c r="B63">
-        <v>151.75</v>
+        <v>151.19999999999999</v>
       </c>
       <c r="C63" s="4">
         <v>145.1</v>
@@ -4950,7 +4942,7 @@
         <v>64</v>
       </c>
       <c r="B64">
-        <v>190.55</v>
+        <v>191.5</v>
       </c>
       <c r="C64" s="4">
         <v>159.55000000000001</v>
@@ -5012,7 +5004,7 @@
         <v>65</v>
       </c>
       <c r="B65">
-        <v>160</v>
+        <v>158.5</v>
       </c>
       <c r="C65" s="4">
         <v>122.9</v>
@@ -5074,7 +5066,7 @@
         <v>66</v>
       </c>
       <c r="B66">
-        <v>879.65</v>
+        <v>879.6</v>
       </c>
       <c r="C66" s="4">
         <v>730.05</v>
@@ -5136,7 +5128,7 @@
         <v>67</v>
       </c>
       <c r="B67">
-        <v>86.3</v>
+        <v>86.25</v>
       </c>
       <c r="C67" s="4">
         <v>56.4</v>
@@ -5198,7 +5190,7 @@
         <v>68</v>
       </c>
       <c r="B68">
-        <v>772.25</v>
+        <v>780.1</v>
       </c>
       <c r="C68" s="4">
         <v>679.05</v>
@@ -5260,7 +5252,7 @@
         <v>69</v>
       </c>
       <c r="B69">
-        <v>1141.3</v>
+        <v>1160.4000000000001</v>
       </c>
       <c r="C69" s="4">
         <v>974.3</v>
@@ -5322,7 +5314,7 @@
         <v>70</v>
       </c>
       <c r="B70">
-        <v>2210.9</v>
+        <v>2236.6999999999998</v>
       </c>
       <c r="C70" s="4">
         <v>1823.15</v>
@@ -5384,7 +5376,7 @@
         <v>71</v>
       </c>
       <c r="B71">
-        <v>404.05</v>
+        <v>406.15</v>
       </c>
       <c r="C71" s="4">
         <v>360.1</v>
@@ -5446,7 +5438,7 @@
         <v>72</v>
       </c>
       <c r="B72">
-        <v>2068.5500000000002</v>
+        <v>2055</v>
       </c>
       <c r="C72" s="4">
         <v>1906.27</v>
@@ -5508,7 +5500,7 @@
         <v>73</v>
       </c>
       <c r="B73">
-        <v>515.20000000000005</v>
+        <v>518.5</v>
       </c>
       <c r="C73" s="4">
         <v>417.65</v>
@@ -5570,7 +5562,7 @@
         <v>74</v>
       </c>
       <c r="B74">
-        <v>3017.3</v>
+        <v>3028.6</v>
       </c>
       <c r="C74" s="4">
         <v>2040.55</v>
@@ -5632,7 +5624,7 @@
         <v>75</v>
       </c>
       <c r="B75">
-        <v>1390.7</v>
+        <v>1450.05</v>
       </c>
       <c r="C75" s="4">
         <v>1253.7</v>
@@ -5694,7 +5686,7 @@
         <v>76</v>
       </c>
       <c r="B76">
-        <v>1492.1</v>
+        <v>1496.5</v>
       </c>
       <c r="C76" s="4">
         <v>1268.4000000000001</v>
@@ -5756,7 +5748,7 @@
         <v>77</v>
       </c>
       <c r="B77">
-        <v>3418.9</v>
+        <v>3444</v>
       </c>
       <c r="C77" s="4">
         <v>2757</v>
@@ -5818,7 +5810,7 @@
         <v>78</v>
       </c>
       <c r="B78">
-        <v>1655.95</v>
+        <v>1652.05</v>
       </c>
       <c r="C78" s="4">
         <v>1489</v>
@@ -5880,7 +5872,7 @@
         <v>79</v>
       </c>
       <c r="B79">
-        <v>644.95000000000005</v>
+        <v>647.79999999999995</v>
       </c>
       <c r="C79" s="4">
         <v>627</v>
@@ -5942,7 +5934,7 @@
         <v>80</v>
       </c>
       <c r="B80">
-        <v>4138.05</v>
+        <v>4277.1499999999996</v>
       </c>
       <c r="C80" s="4">
         <v>3130.1</v>
@@ -6004,7 +5996,7 @@
         <v>81</v>
       </c>
       <c r="B81">
-        <v>580.04999999999995</v>
+        <v>581.95000000000005</v>
       </c>
       <c r="C81" s="4">
         <v>491.65</v>
@@ -6066,7 +6058,7 @@
         <v>82</v>
       </c>
       <c r="B82">
-        <v>269.45</v>
+        <v>268.8</v>
       </c>
       <c r="C82" s="4">
         <v>156.5</v>
@@ -6128,7 +6120,7 @@
         <v>83</v>
       </c>
       <c r="B83">
-        <v>430.7</v>
+        <v>441.35</v>
       </c>
       <c r="C83" s="4">
         <v>300.3</v>
@@ -6190,7 +6182,7 @@
         <v>84</v>
       </c>
       <c r="B84">
-        <v>2577.4</v>
+        <v>2569.4499999999998</v>
       </c>
       <c r="C84" s="4">
         <v>2465</v>
@@ -6252,7 +6244,7 @@
         <v>85</v>
       </c>
       <c r="B85">
-        <v>36815.4</v>
+        <v>36857.300000000003</v>
       </c>
       <c r="C85" s="10">
         <v>34977.699999999997</v>
@@ -6314,7 +6306,7 @@
         <v>86</v>
       </c>
       <c r="B86">
-        <v>216.05</v>
+        <v>219.6</v>
       </c>
       <c r="C86" s="4">
         <v>176.4</v>
@@ -6376,7 +6368,7 @@
         <v>87</v>
       </c>
       <c r="B87">
-        <v>993.05</v>
+        <v>991.15</v>
       </c>
       <c r="C87" s="4">
         <v>914.75</v>
@@ -6438,7 +6430,7 @@
         <v>88</v>
       </c>
       <c r="B88">
-        <v>1388.05</v>
+        <v>1388.85</v>
       </c>
       <c r="C88" s="4">
         <v>1360.2</v>
@@ -6500,7 +6492,7 @@
         <v>89</v>
       </c>
       <c r="B89">
-        <v>541.25</v>
+        <v>544.9</v>
       </c>
       <c r="C89" s="10">
         <v>505.4</v>
@@ -6624,7 +6616,7 @@
         <v>91</v>
       </c>
       <c r="B91">
-        <v>121</v>
+        <v>122.55</v>
       </c>
       <c r="C91" s="4">
         <v>115.1</v>
@@ -6686,7 +6678,7 @@
         <v>92</v>
       </c>
       <c r="B92">
-        <v>83.9</v>
+        <v>84.95</v>
       </c>
       <c r="C92" s="4">
         <v>82.7</v>
@@ -6748,7 +6740,7 @@
         <v>93</v>
       </c>
       <c r="B93">
-        <v>164.05</v>
+        <v>165.85</v>
       </c>
       <c r="C93" s="4">
         <v>132.9</v>
@@ -6810,7 +6802,7 @@
         <v>94</v>
       </c>
       <c r="B94">
-        <v>417.8</v>
+        <v>418.7</v>
       </c>
       <c r="C94" s="4">
         <v>382.65</v>
@@ -6872,7 +6864,7 @@
         <v>95</v>
       </c>
       <c r="B95">
-        <v>458.4</v>
+        <v>459.9</v>
       </c>
       <c r="C95" s="4">
         <v>409</v>
@@ -6934,7 +6926,7 @@
         <v>96</v>
       </c>
       <c r="B96">
-        <v>258.95</v>
+        <v>259</v>
       </c>
       <c r="C96" s="4">
         <v>213</v>
@@ -6996,7 +6988,7 @@
         <v>97</v>
       </c>
       <c r="B97">
-        <v>2577.9499999999998</v>
+        <v>2605</v>
       </c>
       <c r="C97" s="4">
         <v>2547.15</v>
@@ -7058,7 +7050,7 @@
         <v>98</v>
       </c>
       <c r="B98">
-        <v>3082.15</v>
+        <v>3040.55</v>
       </c>
       <c r="C98" s="4">
         <v>2524.1999999999998</v>
@@ -7120,7 +7112,7 @@
         <v>99</v>
       </c>
       <c r="B99">
-        <v>1640.15</v>
+        <v>1665</v>
       </c>
       <c r="C99" s="4">
         <v>1450.05</v>
@@ -7182,7 +7174,7 @@
         <v>100</v>
       </c>
       <c r="B100">
-        <v>214.25</v>
+        <v>217.35</v>
       </c>
       <c r="C100" s="10">
         <v>176.55</v>
@@ -7244,7 +7236,7 @@
         <v>101</v>
       </c>
       <c r="B101">
-        <v>1519.9</v>
+        <v>1513.5</v>
       </c>
       <c r="C101" s="4">
         <v>1393</v>
@@ -7306,7 +7298,7 @@
         <v>102</v>
       </c>
       <c r="B102">
-        <v>811.7</v>
+        <v>812.8</v>
       </c>
       <c r="C102" s="4">
         <v>673.8</v>
@@ -7368,7 +7360,7 @@
         <v>103</v>
       </c>
       <c r="B103">
-        <v>130.55000000000001</v>
+        <v>132.94999999999999</v>
       </c>
       <c r="C103" s="4">
         <v>99.15</v>
@@ -7430,7 +7422,7 @@
         <v>104</v>
       </c>
       <c r="B104">
-        <v>1116.25</v>
+        <v>1134.3</v>
       </c>
       <c r="C104" s="10">
         <v>1041</v>
@@ -7492,7 +7484,7 @@
         <v>105</v>
       </c>
       <c r="B105">
-        <v>941.7</v>
+        <v>940.9</v>
       </c>
       <c r="C105" s="4">
         <v>674</v>
@@ -7554,7 +7546,7 @@
         <v>106</v>
       </c>
       <c r="B106">
-        <v>463.3</v>
+        <v>462.5</v>
       </c>
       <c r="C106" s="4">
         <v>434.15</v>
@@ -7616,7 +7608,7 @@
         <v>107</v>
       </c>
       <c r="B107">
-        <v>731</v>
+        <v>732.5</v>
       </c>
       <c r="C107" s="4">
         <v>642.5</v>
@@ -7678,7 +7670,7 @@
         <v>108</v>
       </c>
       <c r="B108">
-        <v>4052.95</v>
+        <v>4037.3</v>
       </c>
       <c r="C108" s="4">
         <v>3430</v>
@@ -7740,7 +7732,7 @@
         <v>109</v>
       </c>
       <c r="B109">
-        <v>829.8</v>
+        <v>827</v>
       </c>
       <c r="C109" s="4">
         <v>760.65</v>
@@ -7802,7 +7794,7 @@
         <v>110</v>
       </c>
       <c r="B110">
-        <v>522.9</v>
+        <v>526.79999999999995</v>
       </c>
       <c r="C110" s="4">
         <v>506.1</v>
@@ -7864,7 +7856,7 @@
         <v>111</v>
       </c>
       <c r="B111">
-        <v>1820.8</v>
+        <v>1831.45</v>
       </c>
       <c r="C111" s="4">
         <v>1733.7</v>
@@ -7926,7 +7918,7 @@
         <v>112</v>
       </c>
       <c r="B112">
-        <v>165.75</v>
+        <v>168.5</v>
       </c>
       <c r="C112" s="4">
         <v>139</v>
@@ -7988,7 +7980,7 @@
         <v>113</v>
       </c>
       <c r="B113">
-        <v>2502</v>
+        <v>2514.9</v>
       </c>
       <c r="C113" s="10">
         <v>2446.5500000000002</v>
@@ -8050,7 +8042,7 @@
         <v>114</v>
       </c>
       <c r="B114">
-        <v>419.4</v>
+        <v>421.95</v>
       </c>
       <c r="C114" s="4">
         <v>366.05</v>
@@ -8112,7 +8104,7 @@
         <v>115</v>
       </c>
       <c r="B115">
-        <v>567.75</v>
+        <v>571.70000000000005</v>
       </c>
       <c r="C115" s="4">
         <v>452.1</v>
@@ -8174,7 +8166,7 @@
         <v>116</v>
       </c>
       <c r="B116">
-        <v>3545.5</v>
+        <v>3531.6</v>
       </c>
       <c r="C116" s="4">
         <v>3031.05</v>
@@ -8236,7 +8228,7 @@
         <v>117</v>
       </c>
       <c r="B117">
-        <v>5947.5</v>
+        <v>5976.05</v>
       </c>
       <c r="C117" s="4">
         <v>5292.7</v>
@@ -8298,7 +8290,7 @@
         <v>118</v>
       </c>
       <c r="B118">
-        <v>5342.15</v>
+        <v>5365</v>
       </c>
       <c r="C118" s="4">
         <v>4283.05</v>
@@ -8360,7 +8352,7 @@
         <v>119</v>
       </c>
       <c r="B119">
-        <v>1405.25</v>
+        <v>1410.35</v>
       </c>
       <c r="C119" s="4">
         <v>1168.75</v>
@@ -8422,7 +8414,7 @@
         <v>120</v>
       </c>
       <c r="B120">
-        <v>1632.8</v>
+        <v>1636.05</v>
       </c>
       <c r="C120" s="4">
         <v>1533.55</v>
@@ -8484,7 +8476,7 @@
         <v>121</v>
       </c>
       <c r="B121">
-        <v>168.05</v>
+        <v>174.3</v>
       </c>
       <c r="C121" s="4">
         <v>147.15</v>
@@ -8546,7 +8538,7 @@
         <v>122</v>
       </c>
       <c r="B122">
-        <v>531.29999999999995</v>
+        <v>532.70000000000005</v>
       </c>
       <c r="C122" s="4">
         <v>516.04999999999995</v>
@@ -8608,7 +8600,7 @@
         <v>123</v>
       </c>
       <c r="B123">
-        <v>10010.200000000001</v>
+        <v>10057.25</v>
       </c>
       <c r="C123" s="10">
         <v>9832.6</v>
@@ -8670,7 +8662,7 @@
         <v>124</v>
       </c>
       <c r="B124">
-        <v>1117.3499999999999</v>
+        <v>1112.2</v>
       </c>
       <c r="C124" s="4">
         <v>1027</v>
@@ -8732,7 +8724,7 @@
         <v>125</v>
       </c>
       <c r="B125">
-        <v>3061.55</v>
+        <v>3134.5</v>
       </c>
       <c r="C125" s="4">
         <v>2725.2</v>
@@ -8794,7 +8786,7 @@
         <v>126</v>
       </c>
       <c r="B126">
-        <v>1608.4</v>
+        <v>1605</v>
       </c>
       <c r="C126" s="10">
         <v>1540</v>
@@ -8856,7 +8848,7 @@
         <v>127</v>
       </c>
       <c r="B127">
-        <v>930.35</v>
+        <v>945.2</v>
       </c>
       <c r="C127" s="4">
         <v>910.4</v>
@@ -8918,7 +8910,7 @@
         <v>128</v>
       </c>
       <c r="B128">
-        <v>1179.5999999999999</v>
+        <v>1220.5</v>
       </c>
       <c r="C128" s="4">
         <v>1017.55</v>
@@ -8980,7 +8972,7 @@
         <v>129</v>
       </c>
       <c r="B129">
-        <v>109.15</v>
+        <v>110.45</v>
       </c>
       <c r="C129" s="4">
         <v>86.8</v>
@@ -9042,7 +9034,7 @@
         <v>130</v>
       </c>
       <c r="B130">
-        <v>2559.4</v>
+        <v>2593.65</v>
       </c>
       <c r="C130" s="4">
         <v>2210.0500000000002</v>
@@ -9104,7 +9096,7 @@
         <v>131</v>
       </c>
       <c r="B131">
-        <v>131828.4</v>
+        <v>132849.15</v>
       </c>
       <c r="C131" s="4">
         <v>107812.6</v>
@@ -9166,7 +9158,7 @@
         <v>132</v>
       </c>
       <c r="B132">
-        <v>1475.35</v>
+        <v>1495.15</v>
       </c>
       <c r="C132" s="4">
         <v>1290</v>
@@ -9228,7 +9220,7 @@
         <v>133</v>
       </c>
       <c r="B133">
-        <v>130.69999999999999</v>
+        <v>129.75</v>
       </c>
       <c r="C133" s="4">
         <v>90.1</v>
@@ -9290,7 +9282,7 @@
         <v>134</v>
       </c>
       <c r="B134">
-        <v>5243.4</v>
+        <v>5195.2</v>
       </c>
       <c r="C134" s="4">
         <v>4520.5</v>
@@ -9352,7 +9344,7 @@
         <v>135</v>
       </c>
       <c r="B135">
-        <v>3491.05</v>
+        <v>3516.5</v>
       </c>
       <c r="C135" s="4">
         <v>3585.1</v>
@@ -9414,7 +9406,7 @@
         <v>136</v>
       </c>
       <c r="B136">
-        <v>2578.1</v>
+        <v>2561</v>
       </c>
       <c r="C136" s="4">
         <v>2388.31</v>
@@ -9476,7 +9468,7 @@
         <v>137</v>
       </c>
       <c r="B137">
-        <v>210.85</v>
+        <v>212.25</v>
       </c>
       <c r="C137" s="4">
         <v>166.75</v>
@@ -9538,7 +9530,7 @@
         <v>138</v>
       </c>
       <c r="B138">
-        <v>313.35000000000002</v>
+        <v>316.2</v>
       </c>
       <c r="C138" s="4">
         <v>245.95</v>
@@ -9600,7 +9592,7 @@
         <v>139</v>
       </c>
       <c r="B139">
-        <v>1522.1</v>
+        <v>1531.8</v>
       </c>
       <c r="C139" s="4">
         <v>1247.95</v>
@@ -9662,7 +9654,7 @@
         <v>140</v>
       </c>
       <c r="B140">
-        <v>4334.1499999999996</v>
+        <v>4390</v>
       </c>
       <c r="C140" s="4">
         <v>3957.75</v>
@@ -9724,7 +9716,7 @@
         <v>141</v>
       </c>
       <c r="B141">
-        <v>212.1</v>
+        <v>212.3</v>
       </c>
       <c r="C141" s="4">
         <v>188.15</v>
@@ -9786,7 +9778,7 @@
         <v>142</v>
       </c>
       <c r="B142">
-        <v>37138.800000000003</v>
+        <v>36956.550000000003</v>
       </c>
       <c r="C142" s="4">
         <v>36529.550000000003</v>
@@ -9848,7 +9840,7 @@
         <v>143</v>
       </c>
       <c r="B143">
-        <v>921.65</v>
+        <v>932.8</v>
       </c>
       <c r="C143" s="10">
         <v>851</v>
@@ -9910,7 +9902,7 @@
         <v>144</v>
       </c>
       <c r="B144">
-        <v>7381.3</v>
+        <v>7459</v>
       </c>
       <c r="C144" s="4">
         <v>6239.15</v>
@@ -9972,7 +9964,7 @@
         <v>145</v>
       </c>
       <c r="B145">
-        <v>234</v>
+        <v>232.45</v>
       </c>
       <c r="C145" s="4">
         <v>194.4</v>
@@ -10034,7 +10026,7 @@
         <v>146</v>
       </c>
       <c r="B146">
-        <v>390.5</v>
+        <v>396.55</v>
       </c>
       <c r="C146" s="4">
         <v>302</v>
@@ -10096,7 +10088,7 @@
         <v>147</v>
       </c>
       <c r="B147">
-        <v>2709.3</v>
+        <v>2710.75</v>
       </c>
       <c r="C147" s="4">
         <v>2420.85</v>
@@ -10158,7 +10150,7 @@
         <v>148</v>
       </c>
       <c r="B148">
-        <v>3459.4</v>
+        <v>3489.95</v>
       </c>
       <c r="C148" s="4">
         <v>3316.55</v>
@@ -10220,7 +10212,7 @@
         <v>149</v>
       </c>
       <c r="B149">
-        <v>94.4</v>
+        <v>95.15</v>
       </c>
       <c r="C149" s="4">
         <v>75.599999999999994</v>
@@ -10282,7 +10274,7 @@
         <v>150</v>
       </c>
       <c r="B150">
-        <v>4911.8500000000004</v>
+        <v>4075.15</v>
       </c>
       <c r="C150" s="4">
         <v>5092.6499999999996</v>
@@ -10344,7 +10336,7 @@
         <v>151</v>
       </c>
       <c r="B151">
-        <v>239.15</v>
+        <v>241.9</v>
       </c>
       <c r="C151" s="4">
         <v>205.7</v>
@@ -10406,7 +10398,7 @@
         <v>152</v>
       </c>
       <c r="B152">
-        <v>149.85</v>
+        <v>150.94999999999999</v>
       </c>
       <c r="C152" s="4">
         <v>141.6</v>
@@ -10468,7 +10460,7 @@
         <v>153</v>
       </c>
       <c r="B153">
-        <v>974.1</v>
+        <v>974.45</v>
       </c>
       <c r="C153" s="4">
         <v>959.1</v>
@@ -10530,7 +10522,7 @@
         <v>154</v>
       </c>
       <c r="B154">
-        <v>283.55</v>
+        <v>289.14999999999998</v>
       </c>
       <c r="C154" s="4">
         <v>226.75</v>
@@ -10592,7 +10584,7 @@
         <v>155</v>
       </c>
       <c r="B155">
-        <v>420.8</v>
+        <v>424.8</v>
       </c>
       <c r="C155" s="4">
         <v>327.85</v>
@@ -10654,7 +10646,7 @@
         <v>156</v>
       </c>
       <c r="B156">
-        <v>2650.1</v>
+        <v>2667</v>
       </c>
       <c r="C156" s="4">
         <v>2327</v>
@@ -10716,7 +10708,7 @@
         <v>157</v>
       </c>
       <c r="B157">
-        <v>115.05</v>
+        <v>115.2</v>
       </c>
       <c r="C157" s="4">
         <v>87.8</v>
@@ -10778,7 +10770,7 @@
         <v>158</v>
       </c>
       <c r="B158">
-        <v>765.45</v>
+        <v>762.5</v>
       </c>
       <c r="C158" s="4">
         <v>720.8</v>
@@ -10840,7 +10832,7 @@
         <v>159</v>
       </c>
       <c r="B159">
-        <v>1451.45</v>
+        <v>1445.3</v>
       </c>
       <c r="C159" s="4">
         <v>1332.05</v>
@@ -10902,7 +10894,7 @@
         <v>160</v>
       </c>
       <c r="B160">
-        <v>621.75</v>
+        <v>624</v>
       </c>
       <c r="C160" s="4">
         <v>555.15</v>
@@ -10964,7 +10956,7 @@
         <v>161</v>
       </c>
       <c r="B161">
-        <v>26842.15</v>
+        <v>26777.45</v>
       </c>
       <c r="C161" s="4">
         <v>25600</v>
@@ -11026,7 +11018,7 @@
         <v>162</v>
       </c>
       <c r="B162">
-        <v>4180.75</v>
+        <v>4139.8999999999996</v>
       </c>
       <c r="C162" s="4">
         <v>3413.05</v>
@@ -11088,7 +11080,7 @@
         <v>163</v>
       </c>
       <c r="B163">
-        <v>2294.9</v>
+        <v>2312.65</v>
       </c>
       <c r="C163" s="4">
         <v>2324.0500000000002</v>
@@ -11150,7 +11142,7 @@
         <v>164</v>
       </c>
       <c r="B164">
-        <v>1324.85</v>
+        <v>1319.75</v>
       </c>
       <c r="C164" s="4">
         <v>1171</v>
@@ -11212,7 +11204,7 @@
         <v>165</v>
       </c>
       <c r="B165">
-        <v>718.2</v>
+        <v>721.25</v>
       </c>
       <c r="C165" s="4">
         <v>655.35</v>
@@ -11274,7 +11266,7 @@
         <v>166</v>
       </c>
       <c r="B166">
-        <v>715.85</v>
+        <v>737.4</v>
       </c>
       <c r="C166" s="10">
         <v>675.6</v>
@@ -11336,7 +11328,7 @@
         <v>167</v>
       </c>
       <c r="B167">
-        <v>1097.3499999999999</v>
+        <v>1097.4000000000001</v>
       </c>
       <c r="C167" s="4">
         <v>948.1</v>
@@ -11398,7 +11390,7 @@
         <v>168</v>
       </c>
       <c r="B168">
-        <v>1718.4</v>
+        <v>1717.55</v>
       </c>
       <c r="C168" s="4">
         <v>1649.05</v>
@@ -11460,7 +11452,7 @@
         <v>169</v>
       </c>
       <c r="B169">
-        <v>1113.95</v>
+        <v>1115.3499999999999</v>
       </c>
       <c r="C169" s="4">
         <v>906</v>
@@ -11522,7 +11514,7 @@
         <v>170</v>
       </c>
       <c r="B170">
-        <v>808.45</v>
+        <v>812.8</v>
       </c>
       <c r="C170" s="4">
         <v>656.55</v>
@@ -11584,7 +11576,7 @@
         <v>171</v>
       </c>
       <c r="B171">
-        <v>346.45</v>
+        <v>355.1</v>
       </c>
       <c r="C171" s="4">
         <v>257.05</v>
@@ -11646,7 +11638,7 @@
         <v>172</v>
       </c>
       <c r="B172">
-        <v>134.1</v>
+        <v>134.9</v>
       </c>
       <c r="C172" s="4">
         <v>121.5</v>
@@ -11708,7 +11700,7 @@
         <v>173</v>
       </c>
       <c r="B173">
-        <v>3713.05</v>
+        <v>3764.8</v>
       </c>
       <c r="C173" s="4">
         <v>3356.05</v>
@@ -11770,7 +11762,7 @@
         <v>174</v>
       </c>
       <c r="B174">
-        <v>1240.9000000000001</v>
+        <v>1258.75</v>
       </c>
       <c r="C174" s="4">
         <v>1143.5</v>
@@ -11832,7 +11824,7 @@
         <v>175</v>
       </c>
       <c r="B175">
-        <v>3714.45</v>
+        <v>3708.3</v>
       </c>
       <c r="C175" s="4">
         <v>3259.25</v>
@@ -11894,7 +11886,7 @@
         <v>176</v>
       </c>
       <c r="B176">
-        <v>2352.9</v>
+        <v>2445</v>
       </c>
       <c r="C176" s="4">
         <v>2024.65</v>
@@ -11956,7 +11948,7 @@
         <v>177</v>
       </c>
       <c r="B177">
-        <v>1021.85</v>
+        <v>1026.5999999999999</v>
       </c>
       <c r="C177" s="4">
         <v>784.2</v>
@@ -12018,7 +12010,7 @@
         <v>178</v>
       </c>
       <c r="B178">
-        <v>3173.6</v>
+        <v>3195.05</v>
       </c>
       <c r="C178" s="4">
         <v>2491.4</v>
@@ -12080,7 +12072,7 @@
         <v>179</v>
       </c>
       <c r="B179">
-        <v>2020.25</v>
+        <v>2049.15</v>
       </c>
       <c r="C179" s="4">
         <v>1647.05</v>
@@ -12142,7 +12134,7 @@
         <v>180</v>
       </c>
       <c r="B180">
-        <v>1812.95</v>
+        <v>1804.5</v>
       </c>
       <c r="C180" s="4">
         <v>1547</v>
@@ -12204,7 +12196,7 @@
         <v>181</v>
       </c>
       <c r="B181">
-        <v>9776.2000000000007</v>
+        <v>9740.75</v>
       </c>
       <c r="C181" s="4">
         <v>8545.0499999999993</v>
@@ -12266,7 +12258,7 @@
         <v>182</v>
       </c>
       <c r="B182">
-        <v>558.6</v>
+        <v>563</v>
       </c>
       <c r="C182" s="4">
         <v>554.79999999999995</v>
@@ -12328,7 +12320,7 @@
         <v>183</v>
       </c>
       <c r="B183">
-        <v>267.05</v>
+        <v>270.3</v>
       </c>
       <c r="C183" s="4">
         <v>230.75</v>
@@ -12390,7 +12382,7 @@
         <v>184</v>
       </c>
       <c r="B184">
-        <v>1012.15</v>
+        <v>1044.25</v>
       </c>
       <c r="C184" s="4">
         <v>811.15</v>
@@ -12452,7 +12444,7 @@
         <v>185</v>
       </c>
       <c r="B185">
-        <v>1352.25</v>
+        <v>1355</v>
       </c>
       <c r="C185" s="4">
         <v>1293</v>
@@ -12514,7 +12506,7 @@
         <v>186</v>
       </c>
       <c r="B186">
-        <v>453.6</v>
+        <v>455.05</v>
       </c>
       <c r="C186" s="4">
         <v>384.25</v>
@@ -12576,7 +12568,7 @@
         <v>187</v>
       </c>
       <c r="B187">
-        <v>259.8</v>
+        <v>260.45</v>
       </c>
       <c r="C187" s="6">
         <v>242.15</v>

</xml_diff>